<commit_message>
resp, o:N, excretion update
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Physiology/Excretion_rates/F1/worksheets/20220922_Excretion_raw_googledrive.xlsx
+++ b/RAnalysis/Data/Physiology/Excretion_rates/F1/worksheets/20220922_Excretion_raw_googledrive.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.gurr\Documents\Github_repositories\Airradians_multigen_OA\RAnalysis\Data\Physiology\Excretion_rates\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Airradians_multigen_OA\RAnalysis\Data\Physiology\Excretion_rates\F1\worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABBD5CDD-2D66-44F8-A61C-3EAB5908EEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="0" windowWidth="21864" windowHeight="9780"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sept 22 2022" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjZ5xdtDdHeGiRKI/8oJIO9wBzOww=="/>
     </ext>
@@ -34,7 +46,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>First run after 1.5 hours of color development at 40</t>
     </r>
@@ -44,7 +55,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>o</t>
     </r>
@@ -53,7 +63,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t>C</t>
     </r>
@@ -239,11 +248,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -257,52 +265,44 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF24292F"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -314,7 +314,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -351,7 +350,7 @@
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,14 +369,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -471,7 +470,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -526,7 +524,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1D10-49F7-B51D-C79FE123EFE3}"/>
+              <c16:uniqueId val="{00000001-771A-4341-B0F0-76F7B291A032}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -538,11 +536,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1980977520"/>
-        <c:axId val="127793393"/>
+        <c:axId val="83564948"/>
+        <c:axId val="1873249326"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1980977520"/>
+        <c:axId val="83564948"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +561,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" b="1" i="0">
+                  <a:rPr b="1" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -606,12 +604,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127793393"/>
+        <c:crossAx val="1873249326"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127793393"/>
+        <c:axId val="1873249326"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +639,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" b="1" i="0">
+                  <a:rPr b="1" i="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -684,7 +682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1980977520"/>
+        <c:crossAx val="83564948"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -750,7 +748,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="0"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -805,7 +802,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3C3B-4CC0-8C70-2B2BE585950C}"/>
+              <c16:uniqueId val="{00000001-C756-4A67-B41A-D055FD1578A4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -817,11 +814,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86430603"/>
-        <c:axId val="1328139333"/>
+        <c:axId val="2015516408"/>
+        <c:axId val="1290647460"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86430603"/>
+        <c:axId val="2015516408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +851,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -879,12 +875,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1328139333"/>
+        <c:crossAx val="1290647460"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1328139333"/>
+        <c:axId val="1290647460"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +913,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -942,7 +937,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86430603"/>
+        <c:crossAx val="2015516408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -971,7 +966,13 @@
     <xdr:ext cx="4400550" cy="2876550"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="912858126" name="Chart 1"/>
+        <xdr:cNvPr id="912858126" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E1C6936}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -996,7 +997,13 @@
     <xdr:ext cx="4572000" cy="2876550"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1714259683" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="1714259683" name="Chart 2" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000E3862D66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1211,24 +1218,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="12" width="16.6640625" customWidth="1"/>
-    <col min="13" max="25" width="12.6640625" customWidth="1"/>
-    <col min="26" max="36" width="8.6640625" customWidth="1"/>
+    <col min="1" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" customWidth="1"/>
+    <col min="4" max="9" width="10.7265625" customWidth="1"/>
+    <col min="10" max="12" width="16.7265625" customWidth="1"/>
+    <col min="13" max="25" width="12.7265625" customWidth="1"/>
+    <col min="26" max="36" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="16.2">
+    <row r="1" spans="1:24" ht="16.5">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +1254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="14.4">
+    <row r="2" spans="1:24" ht="14.5">
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1278,7 +1285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="14.4">
+    <row r="3" spans="1:24" ht="14.5">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1296,7 +1303,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="14.4">
+    <row r="4" spans="1:24" ht="14.5">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1321,7 +1328,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:24" ht="14.4">
+    <row r="5" spans="1:24" ht="14.5">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1357,7 +1364,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="1:24" ht="14.4">
+    <row r="6" spans="1:24" ht="14.5">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1389,7 +1396,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:24" ht="14.4">
+    <row r="7" spans="1:24" ht="14.5">
       <c r="D7" s="7">
         <v>0.1</v>
       </c>
@@ -1418,7 +1425,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:24" ht="14.4">
+    <row r="8" spans="1:24" ht="14.5">
       <c r="D8" s="7">
         <v>0.2</v>
       </c>
@@ -1447,7 +1454,7 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="1:24" ht="14.4">
+    <row r="9" spans="1:24" ht="14.5">
       <c r="K9" s="1"/>
       <c r="L9" s="2" t="s">
         <v>21</v>
@@ -1462,12 +1469,12 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:24" ht="14.4">
+    <row r="10" spans="1:24" ht="14.5">
       <c r="K10" s="1"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:24" ht="14.4">
+    <row r="11" spans="1:24" ht="14.5">
       <c r="K11" s="1"/>
       <c r="N11" s="6"/>
       <c r="P11" s="3"/>
@@ -1488,7 +1495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="14.4">
+    <row r="12" spans="1:24" ht="14.5">
       <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1550,7 +1557,7 @@
         <v>-8.7194309201083772E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="14.4">
+    <row r="13" spans="1:24" ht="14.5">
       <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1573,7 +1580,10 @@
         <f t="shared" ref="J13:J28" si="3">I13-H13</f>
         <v>1.5277777777777779E-2</v>
       </c>
-      <c r="K13" s="19"/>
+      <c r="K13" s="19">
+        <f t="shared" ref="K13:K14" si="4">22/60</f>
+        <v>0.36666666666666664</v>
+      </c>
       <c r="L13" s="20" t="s">
         <v>40</v>
       </c>
@@ -1592,21 +1602,23 @@
       <c r="R13" s="22">
         <v>201.4</v>
       </c>
-      <c r="S13" s="2"/>
+      <c r="S13" s="11">
+        <v>16.2</v>
+      </c>
       <c r="T13" s="2">
         <f>R13-S13</f>
-        <v>201.4</v>
-      </c>
-      <c r="U13" s="2" t="e">
+        <v>185.20000000000002</v>
+      </c>
+      <c r="U13" s="2">
         <f>(Q13*T13)/K13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V13" s="2" t="e">
+        <v>134.85927272727275</v>
+      </c>
+      <c r="V13" s="2">
         <f>U13/14</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="14.4">
+        <v>9.6328051948051971</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="14.5">
       <c r="D14" s="2" t="s">
         <v>41</v>
       </c>
@@ -1629,7 +1641,10 @@
         <f t="shared" si="3"/>
         <v>1.5277777777777779E-2</v>
       </c>
-      <c r="K14" s="12"/>
+      <c r="K14" s="19">
+        <f t="shared" si="4"/>
+        <v>0.36666666666666664</v>
+      </c>
       <c r="L14" s="20" t="s">
         <v>40</v>
       </c>
@@ -1647,7 +1662,7 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:24" ht="14.4">
+    <row r="15" spans="1:24" ht="14.5">
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="17">
@@ -1660,7 +1675,10 @@
         <f t="shared" si="3"/>
         <v>1.1805555555555569E-2</v>
       </c>
-      <c r="K15" s="12"/>
+      <c r="K15" s="19">
+        <f t="shared" ref="K15:K16" si="5">17/60</f>
+        <v>0.28333333333333333</v>
+      </c>
       <c r="L15" s="20" t="s">
         <v>43</v>
       </c>
@@ -1679,21 +1697,23 @@
       <c r="R15" s="24">
         <v>201.3</v>
       </c>
-      <c r="S15" s="2"/>
+      <c r="S15" s="11">
+        <v>25.2</v>
+      </c>
       <c r="T15" s="2">
         <f>R15-S15</f>
-        <v>201.3</v>
-      </c>
-      <c r="U15" s="2" t="e">
+        <v>176.10000000000002</v>
+      </c>
+      <c r="U15" s="2">
         <f>(Q15*T15)/K15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V15" s="2" t="e">
+        <v>124.92741176470589</v>
+      </c>
+      <c r="V15" s="2">
         <f>U15/14</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="14.4">
+        <v>8.9233865546218496</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="14.5">
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="17">
@@ -1706,7 +1726,10 @@
         <f t="shared" si="3"/>
         <v>1.1805555555555569E-2</v>
       </c>
-      <c r="K16" s="12"/>
+      <c r="K16" s="19">
+        <f t="shared" si="5"/>
+        <v>0.28333333333333333</v>
+      </c>
       <c r="L16" s="20" t="s">
         <v>43</v>
       </c>
@@ -1724,7 +1747,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="6:26" ht="14.4">
+    <row r="17" spans="6:26" ht="14.5">
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="17">
@@ -1737,7 +1760,10 @@
         <f t="shared" si="3"/>
         <v>1.5277777777777779E-2</v>
       </c>
-      <c r="K17" s="12"/>
+      <c r="K17" s="12">
+        <f t="shared" ref="K17:K18" si="6">2/60</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
       <c r="L17" s="20" t="s">
         <v>44</v>
       </c>
@@ -1756,21 +1782,23 @@
       <c r="R17" s="22">
         <v>196.6</v>
       </c>
-      <c r="S17" s="2"/>
+      <c r="S17" s="11">
+        <v>17.3</v>
+      </c>
       <c r="T17" s="2">
         <f>R17-S17</f>
-        <v>196.6</v>
-      </c>
-      <c r="U17" s="2" t="e">
+        <v>179.29999999999998</v>
+      </c>
+      <c r="U17" s="2">
         <f>(Q17*T17)/K17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V17" s="2" t="e">
+        <v>1538.3939999999996</v>
+      </c>
+      <c r="V17" s="2">
         <f>U17/14</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="6:26" ht="14.4">
+        <v>109.88528571428569</v>
+      </c>
+    </row>
+    <row r="18" spans="6:26" ht="14.5">
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="17">
@@ -1783,7 +1811,10 @@
         <f t="shared" si="3"/>
         <v>1.5277777777777779E-2</v>
       </c>
-      <c r="K18" s="12"/>
+      <c r="K18" s="12">
+        <f t="shared" si="6"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
       <c r="L18" s="20" t="s">
         <v>44</v>
       </c>
@@ -1801,7 +1832,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="6:26" ht="14.4">
+    <row r="19" spans="6:26" ht="14.5">
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="17">
@@ -1814,7 +1845,10 @@
         <f t="shared" si="3"/>
         <v>2.3611111111111083E-2</v>
       </c>
-      <c r="K19" s="12"/>
+      <c r="K19" s="12">
+        <f t="shared" ref="K19:K20" si="7">34/60</f>
+        <v>0.56666666666666665</v>
+      </c>
       <c r="L19" s="20" t="s">
         <v>45</v>
       </c>
@@ -1833,20 +1867,23 @@
       <c r="R19" s="25">
         <v>200.6</v>
       </c>
+      <c r="S19" s="25">
+        <v>11.6</v>
+      </c>
       <c r="T19" s="2">
         <f>R19-S19</f>
-        <v>200.6</v>
-      </c>
-      <c r="U19" s="2" t="e">
+        <v>189</v>
+      </c>
+      <c r="U19" s="2">
         <f>(Q19*T19)/K19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V19" s="2" t="e">
+        <v>45.36</v>
+      </c>
+      <c r="V19" s="2">
         <f>U19/14</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="6:26" ht="14.4">
+        <v>3.2399999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="6:26" ht="14.5">
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="17">
@@ -1859,7 +1896,10 @@
         <f t="shared" si="3"/>
         <v>2.3611111111111083E-2</v>
       </c>
-      <c r="K20" s="12"/>
+      <c r="K20" s="12">
+        <f t="shared" si="7"/>
+        <v>0.56666666666666665</v>
+      </c>
       <c r="L20" s="20" t="s">
         <v>45</v>
       </c>
@@ -1882,7 +1922,7 @@
         <v>0.38240941115532412</v>
       </c>
     </row>
-    <row r="21" spans="6:26" ht="14.4">
+    <row r="21" spans="6:26" ht="14.5">
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="17">
@@ -1895,7 +1935,10 @@
         <f t="shared" si="3"/>
         <v>1.8750000000000044E-2</v>
       </c>
-      <c r="K21" s="12"/>
+      <c r="K21" s="19">
+        <f t="shared" ref="K21:K22" si="8">27/60</f>
+        <v>0.45</v>
+      </c>
       <c r="L21" s="20" t="s">
         <v>47</v>
       </c>
@@ -1914,18 +1957,20 @@
       <c r="R21" s="22">
         <v>199.2</v>
       </c>
-      <c r="S21" s="2"/>
+      <c r="S21" s="11">
+        <v>19.600000000000001</v>
+      </c>
       <c r="T21" s="2">
         <f>R21-S21</f>
-        <v>199.2</v>
-      </c>
-      <c r="U21" s="2" t="e">
+        <v>179.6</v>
+      </c>
+      <c r="U21" s="2">
         <f>(Q21*T21)/K21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V21" s="2" t="e">
+        <v>72.638222222222211</v>
+      </c>
+      <c r="V21" s="2">
         <f>U21/14</f>
-        <v>#DIV/0!</v>
+        <v>5.1884444444444435</v>
       </c>
       <c r="Y21" s="2" t="s">
         <v>28</v>
@@ -1948,7 +1993,10 @@
         <f t="shared" si="3"/>
         <v>1.8750000000000044E-2</v>
       </c>
-      <c r="K22" s="12"/>
+      <c r="K22" s="19">
+        <f t="shared" si="8"/>
+        <v>0.45</v>
+      </c>
       <c r="L22" s="20" t="s">
         <v>47</v>
       </c>
@@ -1986,7 +2034,10 @@
         <f t="shared" si="3"/>
         <v>2.9166666666666674E-2</v>
       </c>
-      <c r="K23" s="12"/>
+      <c r="K23" s="12">
+        <f t="shared" ref="K23:K24" si="9">42/60</f>
+        <v>0.7</v>
+      </c>
       <c r="L23" s="20" t="s">
         <v>49</v>
       </c>
@@ -2005,18 +2056,20 @@
       <c r="R23" s="24">
         <v>200.4</v>
       </c>
-      <c r="S23" s="2"/>
+      <c r="S23" s="11">
+        <v>17.7</v>
+      </c>
       <c r="T23" s="2">
         <f>R23-S23</f>
-        <v>200.4</v>
-      </c>
-      <c r="U23" s="2" t="e">
+        <v>182.70000000000002</v>
+      </c>
+      <c r="U23" s="2">
         <f>(Q23*T23)/K23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V23" s="2" t="e">
+        <v>29.232000000000006</v>
+      </c>
+      <c r="V23" s="2">
         <f>U23/14</f>
-        <v>#DIV/0!</v>
+        <v>2.0880000000000005</v>
       </c>
       <c r="Y23" s="2" t="s">
         <v>50</v>
@@ -2039,7 +2092,10 @@
         <f t="shared" si="3"/>
         <v>2.9166666666666674E-2</v>
       </c>
-      <c r="K24" s="12"/>
+      <c r="K24" s="12">
+        <f t="shared" si="9"/>
+        <v>0.7</v>
+      </c>
       <c r="L24" s="20" t="s">
         <v>49</v>
       </c>
@@ -2071,7 +2127,10 @@
         <f t="shared" si="3"/>
         <v>3.0555555555555558E-2</v>
       </c>
-      <c r="K25" s="12"/>
+      <c r="K25" s="12">
+        <f t="shared" ref="K25:K26" si="10">44/60</f>
+        <v>0.73333333333333328</v>
+      </c>
       <c r="L25" s="20" t="s">
         <v>51</v>
       </c>
@@ -2090,18 +2149,20 @@
       <c r="R25" s="22">
         <v>200</v>
       </c>
-      <c r="S25" s="2"/>
+      <c r="S25" s="11">
+        <v>11.8</v>
+      </c>
       <c r="T25" s="2">
         <f>R25-S25</f>
-        <v>200</v>
-      </c>
-      <c r="U25" s="2" t="e">
+        <v>188.2</v>
+      </c>
+      <c r="U25" s="2">
         <f>(Q25*T25)/K25</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V25" s="2" t="e">
+        <v>57.486545454545457</v>
+      </c>
+      <c r="V25" s="2">
         <f>U25/14</f>
-        <v>#DIV/0!</v>
+        <v>4.1061818181818186</v>
       </c>
     </row>
     <row r="26" spans="6:26" ht="15.75" customHeight="1">
@@ -2117,7 +2178,10 @@
         <f t="shared" si="3"/>
         <v>3.0555555555555558E-2</v>
       </c>
-      <c r="K26" s="12"/>
+      <c r="K26" s="12">
+        <f t="shared" si="10"/>
+        <v>0.73333333333333328</v>
+      </c>
       <c r="L26" s="20" t="s">
         <v>51</v>
       </c>
@@ -2148,7 +2212,10 @@
         <f t="shared" si="3"/>
         <v>3.1944444444444442E-2</v>
       </c>
-      <c r="K27" s="12"/>
+      <c r="K27" s="12">
+        <f t="shared" ref="K27:K28" si="11">46/60</f>
+        <v>0.76666666666666672</v>
+      </c>
       <c r="L27" s="20" t="s">
         <v>52</v>
       </c>
@@ -2179,7 +2246,10 @@
         <f t="shared" si="3"/>
         <v>3.1944444444444442E-2</v>
       </c>
-      <c r="K28" s="12"/>
+      <c r="K28" s="12">
+        <f t="shared" si="11"/>
+        <v>0.76666666666666672</v>
+      </c>
       <c r="L28" s="20" t="s">
         <v>52</v>
       </c>
@@ -2223,10 +2293,13 @@
         <v>0.54722222222222228</v>
       </c>
       <c r="J30" s="18">
-        <f t="shared" ref="J30:J45" si="4">I30-H30</f>
+        <f t="shared" ref="J30:J45" si="12">I30-H30</f>
         <v>9.7222222222222987E-3</v>
       </c>
-      <c r="K30" s="12"/>
+      <c r="K30" s="12">
+        <f t="shared" ref="K30:K31" si="13">14/60</f>
+        <v>0.23333333333333334</v>
+      </c>
       <c r="L30" s="20" t="s">
         <v>53</v>
       </c>
@@ -2245,18 +2318,20 @@
       <c r="R30" s="24">
         <v>196.6</v>
       </c>
-      <c r="S30" s="2"/>
+      <c r="S30" s="11">
+        <v>18.3</v>
+      </c>
       <c r="T30" s="2">
         <f>R30-S30</f>
-        <v>196.6</v>
-      </c>
-      <c r="U30" s="2" t="e">
+        <v>178.29999999999998</v>
+      </c>
+      <c r="U30" s="2">
         <f>(Q30*T30)/K30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V30" s="2" t="e">
+        <v>159.70585714285713</v>
+      </c>
+      <c r="V30" s="2">
         <f>U30/14</f>
-        <v>#DIV/0!</v>
+        <v>11.407561224489795</v>
       </c>
     </row>
     <row r="31" spans="6:26" ht="15.75" customHeight="1">
@@ -2269,10 +2344,13 @@
         <v>0.54722222222222228</v>
       </c>
       <c r="J31" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>9.7222222222222987E-3</v>
       </c>
-      <c r="K31" s="12"/>
+      <c r="K31" s="12">
+        <f t="shared" si="13"/>
+        <v>0.23333333333333334</v>
+      </c>
       <c r="L31" s="20" t="s">
         <v>53</v>
       </c>
@@ -2302,10 +2380,13 @@
         <v>0.55138888888888893</v>
       </c>
       <c r="J32" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.4583333333333393E-2</v>
       </c>
-      <c r="K32" s="12"/>
+      <c r="K32" s="12">
+        <f t="shared" ref="K32:K35" si="14">21/60</f>
+        <v>0.35</v>
+      </c>
       <c r="L32" s="20" t="s">
         <v>54</v>
       </c>
@@ -2324,18 +2405,20 @@
       <c r="R32" s="24">
         <v>201.4</v>
       </c>
-      <c r="S32" s="2"/>
+      <c r="S32" s="11">
+        <v>18.7</v>
+      </c>
       <c r="T32" s="2">
         <f>R32-S32</f>
-        <v>201.4</v>
-      </c>
-      <c r="U32" s="2" t="e">
+        <v>182.70000000000002</v>
+      </c>
+      <c r="U32" s="2">
         <f>(Q32*T32)/K32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V32" s="2" t="e">
+        <v>69.426000000000016</v>
+      </c>
+      <c r="V32" s="2">
         <f>U32/14</f>
-        <v>#DIV/0!</v>
+        <v>4.9590000000000014</v>
       </c>
       <c r="W32" s="14"/>
       <c r="X32" s="14"/>
@@ -2350,10 +2433,13 @@
         <v>0.55138888888888893</v>
       </c>
       <c r="J33" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.4583333333333393E-2</v>
       </c>
-      <c r="K33" s="12"/>
+      <c r="K33" s="12">
+        <f t="shared" si="14"/>
+        <v>0.35</v>
+      </c>
       <c r="L33" s="20" t="s">
         <v>54</v>
       </c>
@@ -2383,10 +2469,13 @@
         <v>0.55347222222222225</v>
       </c>
       <c r="J34" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.4583333333333393E-2</v>
       </c>
-      <c r="K34" s="12"/>
+      <c r="K34" s="12">
+        <f t="shared" si="14"/>
+        <v>0.35</v>
+      </c>
       <c r="L34" s="20" t="s">
         <v>55</v>
       </c>
@@ -2405,18 +2494,20 @@
       <c r="R34" s="22">
         <v>200</v>
       </c>
-      <c r="S34" s="2"/>
+      <c r="S34" s="11">
+        <v>18.600000000000001</v>
+      </c>
       <c r="T34" s="2">
         <f>R34-S34</f>
-        <v>200</v>
-      </c>
-      <c r="U34" s="2" t="e">
+        <v>181.4</v>
+      </c>
+      <c r="U34" s="2">
         <f>(Q34*T34)/K34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V34" s="2" t="e">
+        <v>75.151428571428568</v>
+      </c>
+      <c r="V34" s="2">
         <f>U34/14</f>
-        <v>#DIV/0!</v>
+        <v>5.3679591836734692</v>
       </c>
       <c r="W34" s="14"/>
       <c r="X34" s="14"/>
@@ -2431,10 +2522,13 @@
         <v>0.55347222222222225</v>
       </c>
       <c r="J35" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.4583333333333393E-2</v>
       </c>
-      <c r="K35" s="12"/>
+      <c r="K35" s="12">
+        <f t="shared" si="14"/>
+        <v>0.35</v>
+      </c>
       <c r="L35" s="20" t="s">
         <v>55</v>
       </c>
@@ -2460,10 +2554,13 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="J36" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.8055555555555602E-2</v>
       </c>
-      <c r="K36" s="12"/>
+      <c r="K36" s="12">
+        <f t="shared" ref="K36:K37" si="15">26/60</f>
+        <v>0.43333333333333335</v>
+      </c>
       <c r="L36" s="20" t="s">
         <v>56</v>
       </c>
@@ -2482,17 +2579,20 @@
       <c r="R36" s="13">
         <v>200.4</v>
       </c>
+      <c r="S36" s="25">
+        <v>20.7</v>
+      </c>
       <c r="T36" s="30">
         <f>R36-S36</f>
-        <v>200.4</v>
-      </c>
-      <c r="U36" s="2" t="e">
+        <v>179.70000000000002</v>
+      </c>
+      <c r="U36" s="2">
         <f>(Q36*T36)/K36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V36" s="2" t="e">
+        <v>17.831769230769229</v>
+      </c>
+      <c r="V36" s="2">
         <f>AVERAGE(V13:V15,V21:V23,V29:V31)</f>
-        <v>#DIV/0!</v>
+        <v>7.4480394836722565</v>
       </c>
       <c r="W36" s="14"/>
       <c r="X36" s="14"/>
@@ -2507,10 +2607,13 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="J37" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.8055555555555602E-2</v>
       </c>
-      <c r="K37" s="1"/>
+      <c r="K37" s="12">
+        <f t="shared" si="15"/>
+        <v>0.43333333333333335</v>
+      </c>
       <c r="L37" s="20" t="s">
         <v>56</v>
       </c>
@@ -2540,10 +2643,13 @@
         <v>0.55625000000000002</v>
       </c>
       <c r="J38" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.8750000000000044E-2</v>
       </c>
-      <c r="K38" s="1"/>
+      <c r="K38" s="1">
+        <f t="shared" ref="K38:K39" si="16">27/60</f>
+        <v>0.45</v>
+      </c>
       <c r="L38" s="20" t="s">
         <v>57</v>
       </c>
@@ -2562,17 +2668,20 @@
       <c r="R38" s="25">
         <v>200.6</v>
       </c>
+      <c r="S38" s="25">
+        <v>16.899999999999999</v>
+      </c>
       <c r="T38" s="2">
         <f>R38-S38</f>
-        <v>200.6</v>
-      </c>
-      <c r="U38" s="2" t="e">
+        <v>183.7</v>
+      </c>
+      <c r="U38" s="2">
         <f>(Q38*T38)/K38</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V38" s="2" t="e">
+        <v>63.682666666666663</v>
+      </c>
+      <c r="V38" s="2">
         <f>AVERAGE(V15:V17,V23:V25,V31:V33)</f>
-        <v>#DIV/0!</v>
+        <v>25.992370817417871</v>
       </c>
     </row>
     <row r="39" spans="6:24" ht="15.75" customHeight="1">
@@ -2585,10 +2694,13 @@
         <v>0.55625000000000002</v>
       </c>
       <c r="J39" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.8750000000000044E-2</v>
       </c>
-      <c r="K39" s="1"/>
+      <c r="K39" s="1">
+        <f t="shared" si="16"/>
+        <v>0.45</v>
+      </c>
       <c r="L39" s="20" t="s">
         <v>57</v>
       </c>
@@ -2614,10 +2726,13 @@
         <v>0.56041666666666667</v>
       </c>
       <c r="J40" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.1527777777777812E-2</v>
       </c>
-      <c r="K40" s="1"/>
+      <c r="K40" s="1">
+        <f t="shared" ref="K40:K41" si="17">31/60</f>
+        <v>0.51666666666666672</v>
+      </c>
       <c r="L40" s="20" t="s">
         <v>58</v>
       </c>
@@ -2636,17 +2751,20 @@
       <c r="R40" s="25">
         <v>201.3</v>
       </c>
+      <c r="S40" s="25">
+        <v>17.899999999999999</v>
+      </c>
       <c r="T40" s="2">
         <f>R40-S40</f>
-        <v>201.3</v>
-      </c>
-      <c r="U40" s="2" t="e">
+        <v>183.4</v>
+      </c>
+      <c r="U40" s="2">
         <f>(Q40*T40)/K40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V40" s="2" t="e">
+        <v>32.657032258064518</v>
+      </c>
+      <c r="V40" s="2">
         <f>AVERAGE(V17:V19,V25:V27,V33:V35)</f>
-        <v>#DIV/0!</v>
+        <v>30.649856679035242</v>
       </c>
     </row>
     <row r="41" spans="6:24" ht="15.75" customHeight="1">
@@ -2659,10 +2777,13 @@
         <v>0.56041666666666667</v>
       </c>
       <c r="J41" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.1527777777777812E-2</v>
       </c>
-      <c r="K41" s="1"/>
+      <c r="K41" s="1">
+        <f t="shared" si="17"/>
+        <v>0.51666666666666672</v>
+      </c>
       <c r="L41" s="20" t="s">
         <v>58</v>
       </c>
@@ -2688,10 +2809,13 @@
         <v>0.56111111111111112</v>
       </c>
       <c r="J42" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.2916666666666696E-2</v>
       </c>
-      <c r="K42" s="1"/>
+      <c r="K42" s="1">
+        <f t="shared" ref="K42:K43" si="18">33/60</f>
+        <v>0.55000000000000004</v>
+      </c>
       <c r="L42" s="20" t="s">
         <v>59</v>
       </c>
@@ -2710,17 +2834,20 @@
       <c r="R42" s="25">
         <v>199.2</v>
       </c>
+      <c r="S42" s="25">
+        <v>15.7</v>
+      </c>
       <c r="T42" s="2">
         <f>R42-S42</f>
-        <v>199.2</v>
-      </c>
-      <c r="U42" s="2" t="e">
+        <v>183.5</v>
+      </c>
+      <c r="U42" s="2">
         <f>(Q42*T42)/K42</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V42" s="2" t="e">
+        <v>55.383636363636363</v>
+      </c>
+      <c r="V42" s="2">
         <f>AVERAGE(V19:V21,V27:V29,V35:V37)</f>
-        <v>#DIV/0!</v>
+        <v>5.2921613093722328</v>
       </c>
     </row>
     <row r="43" spans="6:24" ht="15.75" customHeight="1">
@@ -2733,10 +2860,13 @@
         <v>0.56111111111111112</v>
       </c>
       <c r="J43" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.2916666666666696E-2</v>
       </c>
-      <c r="K43" s="1"/>
+      <c r="K43" s="1">
+        <f t="shared" si="18"/>
+        <v>0.55000000000000004</v>
+      </c>
       <c r="L43" s="20" t="s">
         <v>59</v>
       </c>
@@ -2762,10 +2892,13 @@
         <v>0.5625</v>
       </c>
       <c r="J44" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.5694444444444464E-2</v>
       </c>
-      <c r="K44" s="1"/>
+      <c r="K44" s="1">
+        <f t="shared" ref="K44:K45" si="19">37/60</f>
+        <v>0.6166666666666667</v>
+      </c>
       <c r="L44" s="20" t="s">
         <v>60</v>
       </c>
@@ -2782,17 +2915,20 @@
       <c r="R44" s="25">
         <v>201.7</v>
       </c>
+      <c r="S44" s="25">
+        <v>5.8</v>
+      </c>
       <c r="T44" s="2">
         <f>R44-S44</f>
-        <v>201.7</v>
-      </c>
-      <c r="U44" s="2" t="e">
+        <v>195.89999999999998</v>
+      </c>
+      <c r="U44" s="2">
         <f>(Q44*T44)/K44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V44" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="V44" s="2">
         <f>AVERAGE(V21:V23,V29:V31,V37:V39)</f>
-        <v>#DIV/0!</v>
+        <v>11.169094121588028</v>
       </c>
     </row>
     <row r="45" spans="6:24" ht="15.75" customHeight="1">
@@ -2805,10 +2941,13 @@
         <v>0.5625</v>
       </c>
       <c r="J45" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2.5694444444444464E-2</v>
       </c>
-      <c r="K45" s="1"/>
+      <c r="K45" s="1">
+        <f t="shared" si="19"/>
+        <v>0.6166666666666667</v>
+      </c>
       <c r="L45" s="20" t="s">
         <v>60</v>
       </c>

</xml_diff>